<commit_message>
Updated number of responses
</commit_message>
<xml_diff>
--- a/reponses.xlsx
+++ b/reponses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie\OneDrive\Uni_Work_Year4\Project\Year-4-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B072FA3A-30FF-4923-8ABF-28E5D41006C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46366564-207A-455E-A381-8A25DBD2563E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{E83F7F5A-7E74-4147-812C-DD764AD0963F}"/>
+    <workbookView xWindow="345" yWindow="3690" windowWidth="16200" windowHeight="8085" xr2:uid="{E83F7F5A-7E74-4147-812C-DD764AD0963F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,14 +115,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,7 +218,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +538,7 @@
   <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +590,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -606,14 +598,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -647,10 +639,10 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>3</v>
       </c>
       <c r="E8" s="4">
@@ -672,11 +664,11 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7">
-        <v>4</v>
+      <c r="C10" s="6">
+        <v>5</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -707,7 +699,7 @@
       </c>
       <c r="F12" s="3">
         <f>SUM(C3:C8)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -722,7 +714,7 @@
       </c>
       <c r="F13" s="4">
         <f>SUM(C9:C14)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -741,7 +733,7 @@
       </c>
       <c r="C15" s="1">
         <f>SUM(C3:C14)</f>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>

</xml_diff>